<commit_message>
Add total remain advance on phieu de nghi tam ung
</commit_message>
<xml_diff>
--- a/src/main/resources/ExportTemplate/PhieuDeNghiTamUngTemplate.xlsx
+++ b/src/main/resources/ExportTemplate/PhieuDeNghiTamUngTemplate.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Working\Projects\GitHub\ael\src\main\resources\ExportTemplate\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dev\workspace\ael\src\main\resources\ExportTemplate\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="34">
   <si>
     <r>
       <t>CÔNG TY TNHH THƯƠNG MẠI – DỊCH VỤ</t>
@@ -199,6 +199,9 @@
   </si>
   <si>
     <t>${advanceDetails.remainAdvance}</t>
+  </si>
+  <si>
+    <t>${totalRemainAdv}</t>
   </si>
 </sst>
 </file>
@@ -769,7 +772,7 @@
   <dimension ref="A2:J19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -890,7 +893,9 @@
       <c r="E15" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="F15" s="10"/>
+      <c r="F15" s="10" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="16" spans="1:10" ht="15.75">
       <c r="C16" s="13" t="s">

</xml_diff>

<commit_message>
thêm tạm ứng admin thêm phiếu thu admin Thanh toán admin ko cần chọn job
</commit_message>
<xml_diff>
--- a/src/main/resources/ExportTemplate/PhieuDeNghiTamUngTemplate.xlsx
+++ b/src/main/resources/ExportTemplate/PhieuDeNghiTamUngTemplate.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Java\ael\src\main\resources\ExportTemplate\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Working\Projects\GitHub\ael\src\main\resources\ExportTemplate\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -772,15 +772,15 @@
   <dimension ref="A2:J19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" activeCellId="4" sqref="E15 F15 F14 E14 E16"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="23.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="23" customWidth="1"/>
-    <col min="4" max="4" width="25.453125" customWidth="1"/>
-    <col min="5" max="5" width="26.453125" customWidth="1"/>
+    <col min="4" max="4" width="25.42578125" customWidth="1"/>
+    <col min="5" max="5" width="26.42578125" customWidth="1"/>
     <col min="6" max="6" width="32" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -799,8 +799,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="15" thickBot="1"/>
-    <row r="6" spans="1:10" ht="15" thickBot="1">
+    <row r="5" spans="1:10" ht="15.75" thickBot="1"/>
+    <row r="6" spans="1:10" ht="15.75" thickBot="1">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
@@ -820,12 +820,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="15.5">
+    <row r="8" spans="1:10" ht="15.75">
       <c r="A8" s="7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="15.5">
+    <row r="9" spans="1:10" ht="15.75">
       <c r="A9" s="8" t="s">
         <v>7</v>
       </c>
@@ -833,7 +833,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="15.5">
+    <row r="10" spans="1:10" ht="15.75">
       <c r="A10" s="8" t="s">
         <v>8</v>
       </c>
@@ -900,7 +900,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="15.5">
+    <row r="16" spans="1:10" ht="15.75">
       <c r="C16" s="13" t="s">
         <v>16</v>
       </c>
@@ -908,7 +908,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="17" spans="2:5" ht="15.5">
+    <row r="17" spans="2:5" ht="15.75">
       <c r="C17" s="13" t="s">
         <v>17</v>
       </c>
@@ -916,12 +916,12 @@
         <v>23</v>
       </c>
     </row>
-    <row r="18" spans="2:5" ht="15.5">
+    <row r="18" spans="2:5" ht="15.75">
       <c r="B18" s="9" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="2:5" ht="15.5">
+    <row r="19" spans="2:5" ht="15.75">
       <c r="B19" s="9" t="s">
         <v>19</v>
       </c>

</xml_diff>

<commit_message>
Add amountVND on refund request + advance request report
</commit_message>
<xml_diff>
--- a/src/main/resources/ExportTemplate/PhieuDeNghiTamUngTemplate.xlsx
+++ b/src/main/resources/ExportTemplate/PhieuDeNghiTamUngTemplate.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\02_projects\kepler_workspace\ael\src\main\resources\ExportTemplate\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14640" windowHeight="4230"/>
   </bookViews>
@@ -19,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="38">
   <si>
     <t>Ad: 308/18 Bình Lợi – Ph.13 – Q.Bình Thạnh – Tp.HCM</t>
   </si>
@@ -149,6 +154,15 @@
   </si>
   <si>
     <t>${refNo}</t>
+  </si>
+  <si>
+    <t>Kế Toán</t>
+  </si>
+  <si>
+    <t>Số tiền bằng chữ:</t>
+  </si>
+  <si>
+    <t>${amountVND}</t>
   </si>
 </sst>
 </file>
@@ -655,7 +669,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -663,10 +677,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:J19"/>
+  <dimension ref="A2:J20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -806,25 +820,36 @@
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C17" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E17" s="15" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C18" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E17" s="2" t="s">
+      <c r="E18" s="2" t="s">
         <v>18</v>
-      </c>
-    </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B18" s="4" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B19" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B20" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C19" s="4" t="s">
+      <c r="C20" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="D19" s="4" t="s">
+      <c r="D20" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E20" s="4" t="s">
         <v>31</v>
       </c>
     </row>

</xml_diff>